<commit_message>
"Quitar lo que no se va a usar"
</commit_message>
<xml_diff>
--- a/samuel/output5.xlsx
+++ b/samuel/output5.xlsx
@@ -415,25 +415,25 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>173.5796321733822</v>
+        <v>160.2659493284493</v>
       </c>
       <c r="C2">
-        <v>0.001275615766644478</v>
+        <v>0.005879875738173723</v>
       </c>
       <c r="D2">
         <v>4.992290249433107</v>
       </c>
       <c r="E2">
-        <v>-0.6029661218471456</v>
+        <v>-0.05798688988061057</v>
       </c>
       <c r="F2">
-        <v>-0.2601557723723369</v>
+        <v>-0.05999019653375162</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>140.1241987179487</v>
+        <v>154.2467948717949</v>
       </c>
       <c r="I2" t="s">
         <v>9</v>

</xml_diff>